<commit_message>
Complete (except making dynamic, will do it.)
</commit_message>
<xml_diff>
--- a/static/Input/Input Data + Sample output.xlsx
+++ b/static/Input/Input Data + Sample output.xlsx
@@ -19,7 +19,7 @@
   <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mg3LE1nWNJFREQSctdQssssvBo6Sw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="" roundtripDataSignature="AMtx7mg3LE1nWNJFREQSctdQssssvBo6Sw=="/>
     </ext>
   </extLst>
 </workbook>
@@ -1170,13 +1170,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1496,11 +1496,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="243644672"/>
-        <c:axId val="243650944"/>
+        <c:axId val="195668224"/>
+        <c:axId val="195678592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="243644672"/>
+        <c:axId val="195668224"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1545,7 +1545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243650944"/>
+        <c:crossAx val="195678592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1553,7 +1553,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243650944"/>
+        <c:axId val="195678592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1610,7 +1610,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243644672"/>
+        <c:crossAx val="195668224"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1886,11 +1886,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="244232192"/>
-        <c:axId val="244234112"/>
+        <c:axId val="196062592"/>
+        <c:axId val="196064768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244232192"/>
+        <c:axId val="196062592"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1935,7 +1935,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244234112"/>
+        <c:crossAx val="196064768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1943,7 +1943,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244234112"/>
+        <c:axId val="196064768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2000,7 +2000,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244232192"/>
+        <c:crossAx val="196062592"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2318,11 +2318,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="244345088"/>
-        <c:axId val="244363648"/>
+        <c:axId val="195794432"/>
+        <c:axId val="195796352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244345088"/>
+        <c:axId val="195794432"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2367,7 +2367,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244363648"/>
+        <c:crossAx val="195796352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2375,7 +2375,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244363648"/>
+        <c:axId val="195796352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2432,7 +2432,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244345088"/>
+        <c:crossAx val="195794432"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2708,11 +2708,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="244813824"/>
-        <c:axId val="244815744"/>
+        <c:axId val="195930752"/>
+        <c:axId val="195937024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244813824"/>
+        <c:axId val="195930752"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2757,7 +2757,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244815744"/>
+        <c:crossAx val="195937024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2765,7 +2765,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244815744"/>
+        <c:axId val="195937024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2822,7 +2822,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244813824"/>
+        <c:crossAx val="195930752"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3161,11 +3161,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="243871104"/>
-        <c:axId val="243873280"/>
+        <c:axId val="196016000"/>
+        <c:axId val="196091904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="243871104"/>
+        <c:axId val="196016000"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3210,7 +3210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243873280"/>
+        <c:crossAx val="196091904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3218,7 +3218,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243873280"/>
+        <c:axId val="196091904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3275,7 +3275,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243871104"/>
+        <c:crossAx val="196016000"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3599,11 +3599,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="244928512"/>
-        <c:axId val="244930432"/>
+        <c:axId val="195302912"/>
+        <c:axId val="195304832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244928512"/>
+        <c:axId val="195302912"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3648,7 +3648,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244930432"/>
+        <c:crossAx val="195304832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3656,7 +3656,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244930432"/>
+        <c:axId val="195304832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3713,7 +3713,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244928512"/>
+        <c:crossAx val="195302912"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3856,11 +3856,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="243935104"/>
-        <c:axId val="243937280"/>
+        <c:axId val="196141056"/>
+        <c:axId val="196142976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="243935104"/>
+        <c:axId val="196141056"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3905,7 +3905,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243937280"/>
+        <c:crossAx val="196142976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3913,7 +3913,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243937280"/>
+        <c:axId val="196142976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3970,7 +3970,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243935104"/>
+        <c:crossAx val="196141056"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4309,11 +4309,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="244982528"/>
-        <c:axId val="244984448"/>
+        <c:axId val="196258048"/>
+        <c:axId val="196276608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244982528"/>
+        <c:axId val="196258048"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4358,7 +4358,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244984448"/>
+        <c:crossAx val="196276608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4366,7 +4366,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244984448"/>
+        <c:axId val="196276608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4423,7 +4423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244982528"/>
+        <c:crossAx val="196258048"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4762,11 +4762,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="245034368"/>
-        <c:axId val="245446144"/>
+        <c:axId val="196338432"/>
+        <c:axId val="196340352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245034368"/>
+        <c:axId val="196338432"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4811,7 +4811,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245446144"/>
+        <c:crossAx val="196340352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4819,7 +4819,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245446144"/>
+        <c:axId val="196340352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4876,7 +4876,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245034368"/>
+        <c:crossAx val="196338432"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5215,11 +5215,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="245566080"/>
-        <c:axId val="245576448"/>
+        <c:axId val="196730240"/>
+        <c:axId val="196732416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245566080"/>
+        <c:axId val="196730240"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5264,7 +5264,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245576448"/>
+        <c:crossAx val="196732416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5272,7 +5272,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245576448"/>
+        <c:axId val="196732416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5329,7 +5329,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245566080"/>
+        <c:crossAx val="196730240"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6109,11 +6109,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="245651328"/>
-        <c:axId val="245657600"/>
+        <c:axId val="196532480"/>
+        <c:axId val="196551040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245651328"/>
+        <c:axId val="196532480"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -6158,7 +6158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245657600"/>
+        <c:crossAx val="196551040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6166,7 +6166,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245657600"/>
+        <c:axId val="196551040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6223,7 +6223,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245651328"/>
+        <c:crossAx val="196532480"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7046,11 +7046,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="245784960"/>
-        <c:axId val="245786880"/>
+        <c:axId val="196616576"/>
+        <c:axId val="196618496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245784960"/>
+        <c:axId val="196616576"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -7095,7 +7095,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245786880"/>
+        <c:crossAx val="196618496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7103,7 +7103,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245786880"/>
+        <c:axId val="196618496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7160,7 +7160,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245784960"/>
+        <c:crossAx val="196616576"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7435,11 +7435,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="219356160"/>
-        <c:axId val="219370624"/>
+        <c:axId val="195412352"/>
+        <c:axId val="195414272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="219356160"/>
+        <c:axId val="195412352"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -7484,7 +7484,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219370624"/>
+        <c:crossAx val="195414272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7492,7 +7492,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="219370624"/>
+        <c:axId val="195414272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7549,7 +7549,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219356160"/>
+        <c:crossAx val="195412352"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8140,11 +8140,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="219689344"/>
-        <c:axId val="219691264"/>
+        <c:axId val="195547136"/>
+        <c:axId val="195549056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="219689344"/>
+        <c:axId val="195547136"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -8189,7 +8189,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219691264"/>
+        <c:crossAx val="195549056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8197,7 +8197,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="219691264"/>
+        <c:axId val="195549056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8254,7 +8254,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219689344"/>
+        <c:crossAx val="195547136"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8572,11 +8572,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="219736704"/>
-        <c:axId val="243606272"/>
+        <c:axId val="195609728"/>
+        <c:axId val="195611648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="219736704"/>
+        <c:axId val="195609728"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -8621,7 +8621,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243606272"/>
+        <c:crossAx val="195611648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8629,7 +8629,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243606272"/>
+        <c:axId val="195611648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8686,7 +8686,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219736704"/>
+        <c:crossAx val="195609728"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9846,8 +9846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9901,7 +9901,7 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="7" t="s">
         <v>306</v>
       </c>
     </row>
@@ -9943,7 +9943,7 @@
         <v>26</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>28</v>
@@ -9993,7 +9993,7 @@
         <v>26</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>28</v>
@@ -10043,7 +10043,7 @@
         <v>26</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>28</v>
@@ -10093,7 +10093,7 @@
         <v>26</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>28</v>
@@ -10143,7 +10143,7 @@
         <v>26</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>28</v>
@@ -10193,7 +10193,7 @@
         <v>26</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>63</v>
@@ -10243,7 +10243,7 @@
         <v>26</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>63</v>
@@ -10293,7 +10293,7 @@
         <v>26</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>63</v>
@@ -10343,7 +10343,7 @@
         <v>26</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>63</v>
@@ -10393,7 +10393,7 @@
         <v>26</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>63</v>
@@ -11093,7 +11093,7 @@
         <v>26</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>94</v>
+        <v>290</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>63</v>
@@ -12834,115 +12834,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="F1" s="7" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="F1" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="K1" s="7" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="K1" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="P1" s="7" t="s">
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="P1" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="U1" s="7" t="s">
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="U1" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
     </row>
     <row r="2" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
     </row>
     <row r="3" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
     </row>
     <row r="4" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
     </row>
     <row r="5" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13923,12 +13923,12 @@
     <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="U1:X4"/>
     <mergeCell ref="D7:J7"/>
     <mergeCell ref="A1:D4"/>
     <mergeCell ref="F1:I4"/>
     <mergeCell ref="K1:N4"/>
     <mergeCell ref="P1:S4"/>
-    <mergeCell ref="U1:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Completed (not dynamuic till now)
</commit_message>
<xml_diff>
--- a/static/Input/Input Data + Sample output.xlsx
+++ b/static/Input/Input Data + Sample output.xlsx
@@ -1173,11 +1173,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1496,11 +1496,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="195668224"/>
-        <c:axId val="195678592"/>
+        <c:axId val="200120576"/>
+        <c:axId val="200130944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195668224"/>
+        <c:axId val="200120576"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1545,7 +1545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195678592"/>
+        <c:crossAx val="200130944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1553,7 +1553,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195678592"/>
+        <c:axId val="200130944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1610,7 +1610,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195668224"/>
+        <c:crossAx val="200120576"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1886,11 +1886,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="196062592"/>
-        <c:axId val="196064768"/>
+        <c:axId val="200256896"/>
+        <c:axId val="200259072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196062592"/>
+        <c:axId val="200256896"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1935,7 +1935,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196064768"/>
+        <c:crossAx val="200259072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1943,7 +1943,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196064768"/>
+        <c:axId val="200259072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2000,7 +2000,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196062592"/>
+        <c:crossAx val="200256896"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2318,11 +2318,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="195794432"/>
-        <c:axId val="195796352"/>
+        <c:axId val="200316416"/>
+        <c:axId val="200318336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195794432"/>
+        <c:axId val="200316416"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2367,7 +2367,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195796352"/>
+        <c:crossAx val="200318336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2375,7 +2375,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195796352"/>
+        <c:axId val="200318336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2432,7 +2432,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195794432"/>
+        <c:crossAx val="200316416"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2708,11 +2708,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="195930752"/>
-        <c:axId val="195937024"/>
+        <c:axId val="200452736"/>
+        <c:axId val="200454912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195930752"/>
+        <c:axId val="200452736"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2757,7 +2757,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195937024"/>
+        <c:crossAx val="200454912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2765,7 +2765,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195937024"/>
+        <c:axId val="200454912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2822,7 +2822,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195930752"/>
+        <c:crossAx val="200452736"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3161,11 +3161,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="196016000"/>
-        <c:axId val="196091904"/>
+        <c:axId val="200529792"/>
+        <c:axId val="200540160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196016000"/>
+        <c:axId val="200529792"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3210,7 +3210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196091904"/>
+        <c:crossAx val="200540160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3218,7 +3218,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196091904"/>
+        <c:axId val="200540160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3275,7 +3275,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196016000"/>
+        <c:crossAx val="200529792"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3599,11 +3599,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="195302912"/>
-        <c:axId val="195304832"/>
+        <c:axId val="199755264"/>
+        <c:axId val="199757184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195302912"/>
+        <c:axId val="199755264"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3648,7 +3648,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195304832"/>
+        <c:crossAx val="199757184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3656,7 +3656,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195304832"/>
+        <c:axId val="199757184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3713,7 +3713,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195302912"/>
+        <c:crossAx val="199755264"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3856,11 +3856,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="196141056"/>
-        <c:axId val="196142976"/>
+        <c:axId val="200593408"/>
+        <c:axId val="200595328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196141056"/>
+        <c:axId val="200593408"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3905,7 +3905,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196142976"/>
+        <c:crossAx val="200595328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3913,7 +3913,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196142976"/>
+        <c:axId val="200595328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3970,7 +3970,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196141056"/>
+        <c:crossAx val="200593408"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4309,11 +4309,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="196258048"/>
-        <c:axId val="196276608"/>
+        <c:axId val="200644864"/>
+        <c:axId val="200659328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196258048"/>
+        <c:axId val="200644864"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4358,7 +4358,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196276608"/>
+        <c:crossAx val="200659328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4366,7 +4366,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196276608"/>
+        <c:axId val="200659328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4423,7 +4423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196258048"/>
+        <c:crossAx val="200644864"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4762,11 +4762,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="196338432"/>
-        <c:axId val="196340352"/>
+        <c:axId val="200794880"/>
+        <c:axId val="200796800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196338432"/>
+        <c:axId val="200794880"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4811,7 +4811,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196340352"/>
+        <c:crossAx val="200796800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4819,7 +4819,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196340352"/>
+        <c:axId val="200796800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4876,7 +4876,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196338432"/>
+        <c:crossAx val="200794880"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5215,11 +5215,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="196730240"/>
-        <c:axId val="196732416"/>
+        <c:axId val="201186688"/>
+        <c:axId val="201188864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196730240"/>
+        <c:axId val="201186688"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5264,7 +5264,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196732416"/>
+        <c:crossAx val="201188864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5272,7 +5272,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196732416"/>
+        <c:axId val="201188864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5329,7 +5329,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196730240"/>
+        <c:crossAx val="201186688"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6109,11 +6109,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="196532480"/>
-        <c:axId val="196551040"/>
+        <c:axId val="200988928"/>
+        <c:axId val="201007488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196532480"/>
+        <c:axId val="200988928"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -6158,7 +6158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196551040"/>
+        <c:crossAx val="201007488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6166,7 +6166,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196551040"/>
+        <c:axId val="201007488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6223,7 +6223,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196532480"/>
+        <c:crossAx val="200988928"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7046,11 +7046,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="196616576"/>
-        <c:axId val="196618496"/>
+        <c:axId val="201068928"/>
+        <c:axId val="201070848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196616576"/>
+        <c:axId val="201068928"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -7095,7 +7095,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196618496"/>
+        <c:crossAx val="201070848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7103,7 +7103,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196618496"/>
+        <c:axId val="201070848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7160,7 +7160,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196616576"/>
+        <c:crossAx val="201068928"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7435,11 +7435,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="195412352"/>
-        <c:axId val="195414272"/>
+        <c:axId val="199868800"/>
+        <c:axId val="199870720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195412352"/>
+        <c:axId val="199868800"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -7484,7 +7484,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195414272"/>
+        <c:crossAx val="199870720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7492,7 +7492,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195414272"/>
+        <c:axId val="199870720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7549,7 +7549,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195412352"/>
+        <c:crossAx val="199868800"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8140,11 +8140,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="195547136"/>
-        <c:axId val="195549056"/>
+        <c:axId val="199990656"/>
+        <c:axId val="200001024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195547136"/>
+        <c:axId val="199990656"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -8189,7 +8189,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195549056"/>
+        <c:crossAx val="200001024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8197,7 +8197,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195549056"/>
+        <c:axId val="200001024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8254,7 +8254,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195547136"/>
+        <c:crossAx val="199990656"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8572,11 +8572,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="195609728"/>
-        <c:axId val="195611648"/>
+        <c:axId val="200066176"/>
+        <c:axId val="200068096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195609728"/>
+        <c:axId val="200066176"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -8621,7 +8621,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195611648"/>
+        <c:crossAx val="200068096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8629,7 +8629,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195611648"/>
+        <c:axId val="200068096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8686,7 +8686,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195609728"/>
+        <c:crossAx val="200066176"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9846,8 +9846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12834,31 +12834,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>263</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>264</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="8" t="s">
         <v>265</v>
       </c>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="8" t="s">
         <v>266</v>
       </c>
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
       <c r="S1" s="9"/>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="8" t="s">
         <v>267</v>
       </c>
       <c r="V1" s="9"/>
@@ -12934,7 +12934,7 @@
     <row r="5" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="10" t="s">
         <v>268</v>
       </c>
       <c r="E7" s="9"/>

</xml_diff>